<commit_message>
fix bug about some strange filenames
</commit_message>
<xml_diff>
--- a/result/stats.xlsx
+++ b/result/stats.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H178"/>
+  <dimension ref="B2:H112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,7 +552,7 @@
         <v>52</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
@@ -618,7 +618,7 @@
         <v>42</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -684,7 +684,7 @@
         <v>271</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13">
@@ -750,7 +750,7 @@
         <v>62</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
@@ -849,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -882,7 +882,7 @@
         <v>5</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -948,7 +948,7 @@
         <v>17</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -981,7 +981,7 @@
         <v>45</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22">
@@ -1047,7 +1047,7 @@
         <v>784</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>570</v>
       </c>
     </row>
     <row r="24">
@@ -1080,7 +1080,7 @@
         <v>33</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
@@ -1146,7 +1146,7 @@
         <v>1244</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="27">
@@ -1179,7 +1179,7 @@
         <v>81</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -1245,7 +1245,7 @@
         <v>45</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30">
@@ -1278,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
@@ -1311,7 +1311,7 @@
         <v>9</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
@@ -1377,7 +1377,7 @@
         <v>12</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
@@ -1472,7 +1472,7 @@
         <v>68</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37">
@@ -1563,7 +1563,7 @@
         <v>5</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -1592,7 +1592,7 @@
         <v>97</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41">
@@ -1708,7 +1708,7 @@
         <v>109</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45">
@@ -1766,7 +1766,7 @@
         <v>238</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47">
@@ -1824,7 +1824,7 @@
         <v>64</v>
       </c>
       <c r="H48" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49">
@@ -2056,7 +2056,7 @@
         <v>18</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57">
@@ -2143,7 +2143,7 @@
         <v>346</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>346</v>
       </c>
     </row>
     <row r="60">
@@ -2230,7 +2230,7 @@
         <v>177</v>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63">
@@ -2288,7 +2288,7 @@
         <v>56</v>
       </c>
       <c r="H64" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65">
@@ -2346,7 +2346,7 @@
         <v>23</v>
       </c>
       <c r="H66" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67">
@@ -2404,7 +2404,7 @@
         <v>11</v>
       </c>
       <c r="H68" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69">
@@ -2468,19 +2468,15 @@
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>Configurations</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>АдминистративныйСервис</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>ManagedApplicationModule</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2492,28 +2488,24 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>Configurations</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ЖурналРегистрации</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>OrdinaryApplicationModule</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2521,32 +2513,28 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>Configurations</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ЖурналРегистрации</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>SessionModule</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2558,10 +2546,10 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>917</v>
+        <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74">
@@ -2572,7 +2560,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>НастройкиПользователя</t>
+          <t>АдминистративныйСервис</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2587,14 +2575,14 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H74" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75">
@@ -2605,7 +2593,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>НастройкиПользователя</t>
+          <t>ЖурналРегистрации</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2620,14 +2608,14 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="H75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -2638,7 +2626,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ПроведениеДокументов</t>
+          <t>ЖурналРегистрации</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2657,10 +2645,10 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>151</v>
+        <v>917</v>
       </c>
       <c r="H76" t="n">
-        <v>0</v>
+        <v>917</v>
       </c>
     </row>
     <row r="77">
@@ -2671,10 +2659,14 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Путеводитель</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr"/>
+          <t>НастройкиПользователя</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E77" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2686,10 +2678,10 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="H77" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -2700,10 +2692,14 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Путеводитель</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr"/>
+          <t>НастройкиПользователя</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E78" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2715,10 +2711,10 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>191</v>
+        <v>65</v>
       </c>
       <c r="H78" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="79">
@@ -2729,7 +2725,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>СписокАктивныхПользователей</t>
+          <t>ПроведениеДокументов</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2748,10 +2744,10 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="H79" t="n">
-        <v>0</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80">
@@ -2762,14 +2758,10 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>УдалениеПомеченныхОбъектов</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>Путеводитель</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2777,14 +2769,14 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>284</v>
+        <v>43</v>
       </c>
       <c r="H80" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -2795,14 +2787,10 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>УправлениеАгрегатамиПродаж</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>Путеводитель</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2814,10 +2802,10 @@
         </is>
       </c>
       <c r="G81" t="n">
-        <v>232</v>
+        <v>191</v>
       </c>
       <c r="H81" t="n">
-        <v>0</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82">
@@ -2828,7 +2816,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>УправлениеНастройкамиФорм</t>
+          <t>СписокАктивныхПользователей</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2847,10 +2835,10 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>415</v>
+        <v>106</v>
       </c>
       <c r="H82" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83">
@@ -2861,7 +2849,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>УправлениеПолнотекстовымПоиском</t>
+          <t>УдалениеПомеченныхОбъектов</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2880,10 +2868,10 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>88</v>
+        <v>284</v>
       </c>
       <c r="H83" t="n">
-        <v>0</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84">
@@ -2894,7 +2882,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>УправлениеСистемойВзаимодействия</t>
+          <t>УправлениеАгрегатамиПродаж</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2909,14 +2897,14 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>173</v>
+        <v>232</v>
       </c>
       <c r="H84" t="n">
-        <v>0</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85">
@@ -2927,7 +2915,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>ЭлектроннаяПочта</t>
+          <t>УправлениеНастройкамиФорм</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2942,14 +2930,14 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>17</v>
+        <v>415</v>
       </c>
       <c r="H85" t="n">
-        <v>19</v>
+        <v>415</v>
       </c>
     </row>
     <row r="86">
@@ -2960,7 +2948,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>ЭлектроннаяПочта</t>
+          <t>УправлениеПолнотекстовымПоиском</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2979,26 +2967,26 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>195</v>
+        <v>88</v>
       </c>
       <c r="H86" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>Documents</t>
+          <t>DataProcessors</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Заказ</t>
+          <t>УправлениеСистемойВзаимодействия</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Продажи</t>
+          <t>Предприятие</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3012,26 +3000,26 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="H87" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>Documents</t>
+          <t>DataProcessors</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Заказ</t>
+          <t>ЭлектроннаяПочта</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Продажи</t>
+          <t>Предприятие</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3041,43 +3029,47 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>323</v>
+        <v>17</v>
       </c>
       <c r="H88" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>Documents</t>
+          <t>DataProcessors</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>НовыйДокумент</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr"/>
+          <t>ЭлектроннаяПочта</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Арипов Никита</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>aripovn@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="H89" t="n">
-        <v>0</v>
+        <v>191</v>
       </c>
     </row>
     <row r="90">
@@ -3088,12 +3080,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>ОперацияПоУчетуТоваров</t>
+          <t>Заказ</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>ТоварныеЗапасы</t>
+          <t>Продажи</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3107,10 +3099,10 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>23</v>
+        <v>162</v>
       </c>
       <c r="H90" t="n">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="91">
@@ -3121,12 +3113,12 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>ОперацияПоУчетуТоваров</t>
+          <t>Заказ</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>ТоварныеЗапасы</t>
+          <t>Продажи</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3140,10 +3132,10 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>90</v>
+        <v>323</v>
       </c>
       <c r="H91" t="n">
-        <v>0</v>
+        <v>312</v>
       </c>
     </row>
     <row r="92">
@@ -3154,29 +3146,25 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Оплата</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Финансы</t>
-        </is>
-      </c>
+          <t>НовыйДокумент</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1C-Company</t>
+          <t>Арипов Никита</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>aripovn@gmail.com</t>
         </is>
       </c>
       <c r="G92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H92" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -3187,12 +3175,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Оплата</t>
+          <t>ОперацияПоУчетуТоваров</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Финансы</t>
+          <t>ТоварныеЗапасы</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3202,14 +3190,14 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="H93" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94">
@@ -3220,12 +3208,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>ПоступлениеДенег</t>
+          <t>ОперацияПоУчетуТоваров</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Финансы</t>
+          <t>ТоварныеЗапасы</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3235,14 +3223,14 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G94" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="H94" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95">
@@ -3253,7 +3241,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>ПоступлениеДенег</t>
+          <t>Оплата</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3268,14 +3256,14 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="H95" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
@@ -3286,12 +3274,12 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>ПриходТовара</t>
+          <t>Оплата</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Закупки</t>
+          <t>Финансы</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3301,14 +3289,14 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="H96" t="n">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97">
@@ -3319,12 +3307,12 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>ПриходТовара</t>
+          <t>ПоступлениеДенег</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Закупки</t>
+          <t>Финансы</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3334,14 +3322,14 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>242</v>
+        <v>7</v>
       </c>
       <c r="H97" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
@@ -3352,12 +3340,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>РасходТовара</t>
+          <t>ПоступлениеДенег</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Продажи</t>
+          <t>Финансы</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3367,14 +3355,14 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="H98" t="n">
-        <v>114</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99">
@@ -3385,12 +3373,12 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>РасходТовара</t>
+          <t>ПриходТовара</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Продажи</t>
+          <t>Закупки</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3400,30 +3388,30 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>688</v>
+        <v>58</v>
       </c>
       <c r="H99" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="inlineStr">
         <is>
-          <t>ExchangePlans</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Мобильные</t>
+          <t>ПриходТовара</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Предприятие</t>
+          <t>Закупки</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3433,28 +3421,32 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G100" t="n">
-        <v>13</v>
+        <v>242</v>
       </c>
       <c r="H100" t="n">
-        <v>13</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>HTTPServices</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>ОписанияТоваров</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr"/>
+          <t>РасходТовара</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Продажи</t>
+        </is>
+      </c>
       <c r="E101" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3466,24 +3458,28 @@
         </is>
       </c>
       <c r="G101" t="n">
-        <v>2</v>
+        <v>129</v>
       </c>
       <c r="H101" t="n">
-        <v>2</v>
+        <v>114</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="inlineStr">
         <is>
-          <t>HTTPServices</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>ОписанияТоваров</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr"/>
+          <t>РасходТовара</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Продажи</t>
+        </is>
+      </c>
       <c r="E102" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3495,24 +3491,28 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>134</v>
+        <v>688</v>
       </c>
       <c r="H102" t="n">
-        <v>67</v>
+        <v>680</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>HTTPServices</t>
+          <t>ExchangePlans</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Товары</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr"/>
+          <t>Мобильные</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E103" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3524,10 +3524,10 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H103" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Товары</t>
+          <t>ОписанияТоваров</t>
         </is>
       </c>
       <c r="D104" t="inlineStr"/>
@@ -3549,25 +3549,25 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>432</v>
+        <v>2</v>
       </c>
       <c r="H104" t="n">
-        <v>216</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>ManagedApplicationModule</t>
+          <t>HTTPServices</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>bsl</t>
+          <t>ОписанияТоваров</t>
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
@@ -3582,21 +3582,21 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="H105" t="n">
-        <v>12</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>OrdinaryApplicationModule</t>
+          <t>HTTPServices</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>bsl</t>
+          <t>Товары</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
@@ -3607,32 +3607,28 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H106" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="inlineStr">
         <is>
-          <t>Reports</t>
+          <t>HTTPServices</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>ОстаткиТоваровНаСкладах</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Закупки, Продажи, ТоварныеЗапасы</t>
-        </is>
-      </c>
+          <t>Товары</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3640,14 +3636,14 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>1</v>
+        <v>432</v>
       </c>
       <c r="H107" t="n">
-        <v>1</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108">
@@ -3673,28 +3669,32 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G108" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="inlineStr">
         <is>
-          <t>SessionModule</t>
+          <t>Reports</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>bsl</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr"/>
+          <t>ОстаткиТоваровНаСкладах</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, ТоварныеЗапасы</t>
+        </is>
+      </c>
       <c r="E109" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3706,10 +3706,10 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H109" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110">
@@ -3797,1920 +3797,6 @@
       </c>
       <c r="H112" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>АдминистративныйСервис</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G113" t="n">
-        <v>0</v>
-      </c>
-      <c r="H113" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>АдминистративныйСервис</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr"/>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G114" t="n">
-        <v>0</v>
-      </c>
-      <c r="H114" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Взаиморасчеты</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G115" t="n">
-        <v>0</v>
-      </c>
-      <c r="H115" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>ВходящиеПисьма</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr"/>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G116" t="n">
-        <v>0</v>
-      </c>
-      <c r="H116" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>ЖурналРегистрации</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G117" t="n">
-        <v>0</v>
-      </c>
-      <c r="H117" t="n">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>ЖурналРегистрации</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G118" t="n">
-        <v>0</v>
-      </c>
-      <c r="H118" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Заказ</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr"/>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G119" t="n">
-        <v>0</v>
-      </c>
-      <c r="H119" t="n">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>Заказ</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr"/>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G120" t="n">
-        <v>0</v>
-      </c>
-      <c r="H120" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>ИсходящиеПисьма</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G121" t="n">
-        <v>0</v>
-      </c>
-      <c r="H121" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>ИсходящиеПисьма</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr"/>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G122" t="n">
-        <v>0</v>
-      </c>
-      <c r="H122" t="n">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Контрагенты</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr"/>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G123" t="n">
-        <v>0</v>
-      </c>
-      <c r="H123" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>Контрагенты</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>ManagerModule</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr"/>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G124" t="n">
-        <v>0</v>
-      </c>
-      <c r="H124" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>Контрагенты</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G125" t="n">
-        <v>0</v>
-      </c>
-      <c r="H125" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>НастроитьСканерШтрихКодов</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>CommandModule</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr"/>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G126" t="n">
-        <v>0</v>
-      </c>
-      <c r="H126" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>НастройкаPushУведомлений</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr"/>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G127" t="n">
-        <v>0</v>
-      </c>
-      <c r="H127" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>НастройкиПользователя</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr"/>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G128" t="n">
-        <v>0</v>
-      </c>
-      <c r="H128" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>НастройкиТорговогоОборудования</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr"/>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G129" t="n">
-        <v>0</v>
-      </c>
-      <c r="H129" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>ОбменМобильныеОбщее</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr"/>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G130" t="n">
-        <v>0</v>
-      </c>
-      <c r="H130" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>ОбменМобильныеПереопределяемый</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr"/>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G131" t="n">
-        <v>0</v>
-      </c>
-      <c r="H131" t="n">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>ОбщиеНастройки</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr"/>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G132" t="n">
-        <v>0</v>
-      </c>
-      <c r="H132" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>ОперацияПоУчетуТоваров</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr"/>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G133" t="n">
-        <v>0</v>
-      </c>
-      <c r="H133" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>ОперацияПоУчетуТоваров</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr"/>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G134" t="n">
-        <v>0</v>
-      </c>
-      <c r="H134" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Оплата</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr"/>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G135" t="n">
-        <v>0</v>
-      </c>
-      <c r="H135" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>Оплата</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr"/>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G136" t="n">
-        <v>0</v>
-      </c>
-      <c r="H136" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>Организации</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D137" t="inlineStr"/>
-      <c r="E137" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G137" t="n">
-        <v>0</v>
-      </c>
-      <c r="H137" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>ОстаткиТоваровНаСкладах</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr"/>
-      <c r="E138" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G138" t="n">
-        <v>0</v>
-      </c>
-      <c r="H138" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Пользователи</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr"/>
-      <c r="E139" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G139" t="n">
-        <v>0</v>
-      </c>
-      <c r="H139" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>Пользователи</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr"/>
-      <c r="E140" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G140" t="n">
-        <v>0</v>
-      </c>
-      <c r="H140" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>ПоступлениеДенег</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr"/>
-      <c r="E141" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F141" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G141" t="n">
-        <v>0</v>
-      </c>
-      <c r="H141" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>ПоступлениеДенег</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr"/>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F142" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G142" t="n">
-        <v>0</v>
-      </c>
-      <c r="H142" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>ПриходТовара</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr"/>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F143" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G143" t="n">
-        <v>0</v>
-      </c>
-      <c r="H143" t="n">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>ПриходТовара</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>ManagerModule</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr"/>
-      <c r="E144" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G144" t="n">
-        <v>0</v>
-      </c>
-      <c r="H144" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>ПриходТовара</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr"/>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G145" t="n">
-        <v>0</v>
-      </c>
-      <c r="H145" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>ПроведениеДокументов</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr"/>
-      <c r="E146" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G146" t="n">
-        <v>0</v>
-      </c>
-      <c r="H146" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>ПроведениеДокументов</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr"/>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G147" t="n">
-        <v>0</v>
-      </c>
-      <c r="H147" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Путеводитель</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr"/>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G148" t="n">
-        <v>0</v>
-      </c>
-      <c r="H148" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Путеводитель</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr"/>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G149" t="n">
-        <v>0</v>
-      </c>
-      <c r="H149" t="n">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>РаботаСПолнотекстовымПоиском</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr"/>
-      <c r="E150" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G150" t="n">
-        <v>0</v>
-      </c>
-      <c r="H150" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>РаботаСПочтой</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr"/>
-      <c r="E151" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F151" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G151" t="n">
-        <v>0</v>
-      </c>
-      <c r="H151" t="n">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>РаботаСТорговымОборудованием</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr"/>
-      <c r="E152" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F152" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G152" t="n">
-        <v>0</v>
-      </c>
-      <c r="H152" t="n">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>РаботаСХранилищемОбщихНастроек</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr"/>
-      <c r="E153" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F153" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G153" t="n">
-        <v>0</v>
-      </c>
-      <c r="H153" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>РасходТовара</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="D154" t="inlineStr"/>
-      <c r="E154" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F154" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G154" t="n">
-        <v>0</v>
-      </c>
-      <c r="H154" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>РасходТовара</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr"/>
-      <c r="E155" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G155" t="n">
-        <v>0</v>
-      </c>
-      <c r="H155" t="n">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>РасходТовара</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F156" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G156" t="n">
-        <v>0</v>
-      </c>
-      <c r="H156" t="n">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>РасчетныеСчетаКонтрагентов</t>
-        </is>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D157" t="inlineStr"/>
-      <c r="E157" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F157" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G157" t="n">
-        <v>0</v>
-      </c>
-      <c r="H157" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>РегламентныеЗаданияАгрегатов</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D158" t="inlineStr"/>
-      <c r="E158" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G158" t="n">
-        <v>0</v>
-      </c>
-      <c r="H158" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>СервисныеМеханизмы</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>Module</t>
-        </is>
-      </c>
-      <c r="D159" t="inlineStr"/>
-      <c r="E159" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F159" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G159" t="n">
-        <v>0</v>
-      </c>
-      <c r="H159" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>Склады</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>ManagerModule</t>
-        </is>
-      </c>
-      <c r="D160" t="inlineStr"/>
-      <c r="E160" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F160" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G160" t="n">
-        <v>0</v>
-      </c>
-      <c r="H160" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>СписокАктивныхПользователей</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D161" t="inlineStr"/>
-      <c r="E161" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F161" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G161" t="n">
-        <v>0</v>
-      </c>
-      <c r="H161" t="n">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>Товары</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr"/>
-      <c r="E162" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F162" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G162" t="n">
-        <v>0</v>
-      </c>
-      <c r="H162" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>Товары</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr"/>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G163" t="n">
-        <v>0</v>
-      </c>
-      <c r="H163" t="n">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>Товары</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr"/>
-      <c r="E164" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F164" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G164" t="n">
-        <v>0</v>
-      </c>
-      <c r="H164" t="n">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>УдалениеПомеченныхОбъектов</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr"/>
-      <c r="E165" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F165" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G165" t="n">
-        <v>0</v>
-      </c>
-      <c r="H165" t="n">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>УправлениеАгрегатамиПродаж</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr"/>
-      <c r="E166" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F166" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G166" t="n">
-        <v>0</v>
-      </c>
-      <c r="H166" t="n">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>УправлениеНастройкамиФорм</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr"/>
-      <c r="E167" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F167" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G167" t="n">
-        <v>0</v>
-      </c>
-      <c r="H167" t="n">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>УправлениеНастройкамиФорм</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr"/>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G168" t="n">
-        <v>0</v>
-      </c>
-      <c r="H168" t="n">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>УправлениеПолнотекстовымПоиском</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr"/>
-      <c r="E169" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F169" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G169" t="n">
-        <v>0</v>
-      </c>
-      <c r="H169" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>УстановитьВидимостьОбъектовЧерезODataAPI</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>CommandModule</t>
-        </is>
-      </c>
-      <c r="D170" t="inlineStr"/>
-      <c r="E170" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F170" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G170" t="n">
-        <v>0</v>
-      </c>
-      <c r="H170" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>УстановитьРасширениеРаботыСКриптографией</t>
-        </is>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>CommandModule</t>
-        </is>
-      </c>
-      <c r="D171" t="inlineStr"/>
-      <c r="E171" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F171" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G171" t="n">
-        <v>0</v>
-      </c>
-      <c r="H171" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>УстановитьРасширениеРаботыСФайлами</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>CommandModule</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr"/>
-      <c r="E172" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F172" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G172" t="n">
-        <v>0</v>
-      </c>
-      <c r="H172" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>УстановитьСканерШтрихкодов</t>
-        </is>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>CommandModule</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr"/>
-      <c r="E173" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F173" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G173" t="n">
-        <v>0</v>
-      </c>
-      <c r="H173" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>ФормаПодбора</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D174" t="inlineStr"/>
-      <c r="E174" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F174" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G174" t="n">
-        <v>0</v>
-      </c>
-      <c r="H174" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>ХранилищеВариантовОтчетов</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>Command</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr"/>
-      <c r="E175" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F175" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G175" t="n">
-        <v>0</v>
-      </c>
-      <c r="H175" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>ХранимыеФайлы</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr"/>
-      <c r="E176" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F176" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G176" t="n">
-        <v>0</v>
-      </c>
-      <c r="H176" t="n">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>ХранимыеФайлы</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>ObjectModule</t>
-        </is>
-      </c>
-      <c r="D177" t="inlineStr"/>
-      <c r="E177" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F177" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G177" t="n">
-        <v>0</v>
-      </c>
-      <c r="H177" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>ЭлектроннаяПочта</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>Form</t>
-        </is>
-      </c>
-      <c r="D178" t="inlineStr"/>
-      <c r="E178" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F178" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G178" t="n">
-        <v>0</v>
-      </c>
-      <c r="H178" t="n">
-        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
little refactoring in html and comment bug
</commit_message>
<xml_diff>
--- a/result/stats.xlsx
+++ b/result/stats.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H112"/>
+  <dimension ref="B2:H109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Коммиты с 2016-01-01 по 2024-03-16</t>
+          <t>Коммиты с 2016-01-01 по 2024-03-18</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
         <v>52</v>
       </c>
       <c r="H8" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -618,7 +618,7 @@
         <v>42</v>
       </c>
       <c r="H10" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -684,7 +684,7 @@
         <v>271</v>
       </c>
       <c r="H12" t="n">
-        <v>271</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -750,7 +750,7 @@
         <v>62</v>
       </c>
       <c r="H14" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -849,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="H17" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -882,7 +882,7 @@
         <v>5</v>
       </c>
       <c r="H18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -948,7 +948,7 @@
         <v>17</v>
       </c>
       <c r="H20" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -981,7 +981,7 @@
         <v>45</v>
       </c>
       <c r="H21" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1047,7 +1047,7 @@
         <v>784</v>
       </c>
       <c r="H23" t="n">
-        <v>570</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1080,7 +1080,7 @@
         <v>33</v>
       </c>
       <c r="H24" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1146,7 +1146,7 @@
         <v>1244</v>
       </c>
       <c r="H26" t="n">
-        <v>1218</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1179,7 +1179,7 @@
         <v>81</v>
       </c>
       <c r="H27" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1245,7 +1245,7 @@
         <v>45</v>
       </c>
       <c r="H29" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1278,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="H30" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1311,7 +1311,7 @@
         <v>9</v>
       </c>
       <c r="H31" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1377,7 +1377,7 @@
         <v>12</v>
       </c>
       <c r="H33" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1472,7 +1472,7 @@
         <v>68</v>
       </c>
       <c r="H36" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1563,7 +1563,7 @@
         <v>5</v>
       </c>
       <c r="H39" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1592,7 +1592,7 @@
         <v>97</v>
       </c>
       <c r="H40" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1708,7 +1708,7 @@
         <v>109</v>
       </c>
       <c r="H44" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1766,7 +1766,7 @@
         <v>238</v>
       </c>
       <c r="H46" t="n">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1824,7 +1824,7 @@
         <v>64</v>
       </c>
       <c r="H48" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2056,7 +2056,7 @@
         <v>18</v>
       </c>
       <c r="H56" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2143,7 +2143,7 @@
         <v>346</v>
       </c>
       <c r="H59" t="n">
-        <v>346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2230,7 +2230,7 @@
         <v>177</v>
       </c>
       <c r="H62" t="n">
-        <v>171</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2288,7 +2288,7 @@
         <v>56</v>
       </c>
       <c r="H64" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2346,7 +2346,7 @@
         <v>23</v>
       </c>
       <c r="H66" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2404,7 +2404,7 @@
         <v>11</v>
       </c>
       <c r="H68" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2468,15 +2468,19 @@
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>Configurations</t>
+          <t>DataProcessors</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>ManagedApplicationModule</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr"/>
+          <t>АдминистративныйСервис</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E71" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2488,24 +2492,28 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H71" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>Configurations</t>
+          <t>DataProcessors</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>OrdinaryApplicationModule</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
+          <t>ЖурналРегистрации</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2513,28 +2521,32 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>Configurations</t>
+          <t>DataProcessors</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SessionModule</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr"/>
+          <t>ЖурналРегистрации</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E73" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2546,10 +2558,10 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>917</v>
       </c>
       <c r="H73" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2560,7 +2572,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>АдминистративныйСервис</t>
+          <t>НастройкиПользователя</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2575,14 +2587,14 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H74" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -2593,7 +2605,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ЖурналРегистрации</t>
+          <t>НастройкиПользователя</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2608,14 +2620,14 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="H75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2626,7 +2638,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ЖурналРегистрации</t>
+          <t>ПроведениеДокументов</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2645,10 +2657,10 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>917</v>
+        <v>151</v>
       </c>
       <c r="H76" t="n">
-        <v>917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2659,14 +2671,10 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>НастройкиПользователя</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>Путеводитель</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2678,10 +2686,10 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="H77" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -2692,14 +2700,10 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>НастройкиПользователя</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>Путеводитель</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2711,10 +2715,10 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="H78" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2725,7 +2729,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ПроведениеДокументов</t>
+          <t>СписокАктивныхПользователей</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2744,10 +2748,10 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>151</v>
+        <v>106</v>
       </c>
       <c r="H79" t="n">
-        <v>151</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2758,10 +2762,14 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Путеводитель</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr"/>
+          <t>УдалениеПомеченныхОбъектов</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E80" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2769,14 +2777,14 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>43</v>
+        <v>284</v>
       </c>
       <c r="H80" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2787,10 +2795,14 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Путеводитель</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr"/>
+          <t>УправлениеАгрегатамиПродаж</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -2802,10 +2814,10 @@
         </is>
       </c>
       <c r="G81" t="n">
-        <v>191</v>
+        <v>232</v>
       </c>
       <c r="H81" t="n">
-        <v>184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2816,7 +2828,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>СписокАктивныхПользователей</t>
+          <t>УправлениеНастройкамиФорм</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2835,10 +2847,10 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>106</v>
+        <v>415</v>
       </c>
       <c r="H82" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2849,7 +2861,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>УдалениеПомеченныхОбъектов</t>
+          <t>УправлениеПолнотекстовымПоиском</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2868,10 +2880,10 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>284</v>
+        <v>88</v>
       </c>
       <c r="H83" t="n">
-        <v>284</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2882,7 +2894,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>УправлениеАгрегатамиПродаж</t>
+          <t>УправлениеСистемойВзаимодействия</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2897,14 +2909,14 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>232</v>
+        <v>173</v>
       </c>
       <c r="H84" t="n">
-        <v>232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2915,7 +2927,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>УправлениеНастройкамиФорм</t>
+          <t>ЭлектроннаяПочта</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2930,14 +2942,14 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>415</v>
+        <v>17</v>
       </c>
       <c r="H85" t="n">
-        <v>415</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86">
@@ -2948,7 +2960,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>УправлениеПолнотекстовымПоиском</t>
+          <t>ЭлектроннаяПочта</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2967,26 +2979,26 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="H86" t="n">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>УправлениеСистемойВзаимодействия</t>
+          <t>Заказ</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Предприятие</t>
+          <t>Продажи</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3000,26 +3012,26 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>ЭлектроннаяПочта</t>
+          <t>Заказ</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Предприятие</t>
+          <t>Продажи</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3029,47 +3041,43 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>17</v>
+        <v>323</v>
       </c>
       <c r="H88" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>ЭлектроннаяПочта</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>НовыйДокумент</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1C-Company</t>
+          <t>Арипов Никита</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>aripovn@gmail.com</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="H89" t="n">
-        <v>191</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -3080,12 +3088,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Заказ</t>
+          <t>ОперацияПоУчетуТоваров</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Продажи</t>
+          <t>ТоварныеЗапасы</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3099,10 +3107,10 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>162</v>
+        <v>23</v>
       </c>
       <c r="H90" t="n">
-        <v>70</v>
+        <v>23</v>
       </c>
     </row>
     <row r="91">
@@ -3113,12 +3121,12 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Заказ</t>
+          <t>ОперацияПоУчетуТоваров</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Продажи</t>
+          <t>ТоварныеЗапасы</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3132,10 +3140,10 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>323</v>
+        <v>90</v>
       </c>
       <c r="H91" t="n">
-        <v>312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3146,25 +3154,29 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>НовыйДокумент</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr"/>
+          <t>Оплата</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Финансы</t>
+        </is>
+      </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Арипов Никита</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>aripovn@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G92" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H92" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
@@ -3175,12 +3187,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>ОперацияПоУчетуТоваров</t>
+          <t>Оплата</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>ТоварныеЗапасы</t>
+          <t>Финансы</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3190,14 +3202,14 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="H93" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -3208,12 +3220,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>ОперацияПоУчетуТоваров</t>
+          <t>ПоступлениеДенег</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>ТоварныеЗапасы</t>
+          <t>Финансы</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3223,14 +3235,14 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G94" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="H94" t="n">
-        <v>90</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
@@ -3241,7 +3253,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Оплата</t>
+          <t>ПоступлениеДенег</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3256,14 +3268,14 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H95" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3274,12 +3286,12 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Оплата</t>
+          <t>ПриходТовара</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Финансы</t>
+          <t>Закупки</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3289,14 +3301,14 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="H96" t="n">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="97">
@@ -3307,12 +3319,12 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>ПоступлениеДенег</t>
+          <t>ПриходТовара</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Финансы</t>
+          <t>Закупки</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3322,14 +3334,14 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>7</v>
+        <v>242</v>
       </c>
       <c r="H97" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -3340,12 +3352,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>ПоступлениеДенег</t>
+          <t>РасходТовара</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Финансы</t>
+          <t>Продажи</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3355,14 +3367,14 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="H98" t="n">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99">
@@ -3373,12 +3385,12 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>ПриходТовара</t>
+          <t>РасходТовара</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Закупки</t>
+          <t>Продажи</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3388,30 +3400,30 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>58</v>
+        <v>688</v>
       </c>
       <c r="H99" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="inlineStr">
         <is>
-          <t>Documents</t>
+          <t>ExchangePlans</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>ПриходТовара</t>
+          <t>Мобильные</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Закупки</t>
+          <t>Предприятие</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3421,32 +3433,28 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G100" t="n">
-        <v>242</v>
+        <v>13</v>
       </c>
       <c r="H100" t="n">
-        <v>230</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>Documents</t>
+          <t>HTTPServices</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>РасходТовара</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Продажи</t>
-        </is>
-      </c>
+          <t>ОписанияТоваров</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3458,28 +3466,24 @@
         </is>
       </c>
       <c r="G101" t="n">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="H101" t="n">
-        <v>114</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="inlineStr">
         <is>
-          <t>Documents</t>
+          <t>HTTPServices</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>РасходТовара</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Продажи</t>
-        </is>
-      </c>
+          <t>ОписанияТоваров</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3491,28 +3495,24 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>688</v>
+        <v>134</v>
       </c>
       <c r="H102" t="n">
-        <v>680</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>ExchangePlans</t>
+          <t>HTTPServices</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Мобильные</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Предприятие</t>
-        </is>
-      </c>
+          <t>Товары</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3524,10 +3524,10 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H103" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>ОписанияТоваров</t>
+          <t>Товары</t>
         </is>
       </c>
       <c r="D104" t="inlineStr"/>
@@ -3549,28 +3549,32 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>2</v>
+        <v>432</v>
       </c>
       <c r="H104" t="n">
-        <v>2</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>HTTPServices</t>
+          <t>Reports</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>ОписанияТоваров</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr"/>
+          <t>ОстаткиТоваровНаСкладах</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, ТоварныеЗапасы</t>
+        </is>
+      </c>
       <c r="E105" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3578,28 +3582,32 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>shan@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>134</v>
+        <v>1</v>
       </c>
       <c r="H105" t="n">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>HTTPServices</t>
+          <t>Reports</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Товары</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr"/>
+          <t>ОстаткиТоваровНаСкладах</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, ТоварныеЗапасы</t>
+        </is>
+      </c>
       <c r="E106" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3607,25 +3615,25 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>register.github@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H106" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="inlineStr">
         <is>
-          <t>HTTPServices</t>
+          <t>SettingsStorages</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Товары</t>
+          <t>ХранилищеВариантовОтчетов</t>
         </is>
       </c>
       <c r="D107" t="inlineStr"/>
@@ -3640,28 +3648,24 @@
         </is>
       </c>
       <c r="G107" t="n">
-        <v>432</v>
+        <v>1024</v>
       </c>
       <c r="H107" t="n">
-        <v>216</v>
+        <v>512</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="inlineStr">
         <is>
-          <t>Reports</t>
+          <t>WebServices</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>ОстаткиТоваровНаСкладах</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Закупки, Продажи, ТоварныеЗапасы</t>
-        </is>
-      </c>
+          <t>MAExchange</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3673,28 +3677,24 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="H108" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="inlineStr">
         <is>
-          <t>Reports</t>
+          <t>WebServices</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>ОстаткиТоваровНаСкладах</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Закупки, Продажи, ТоварныеЗапасы</t>
-        </is>
-      </c>
+          <t>MAExchange</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr">
         <is>
           <t>1C-Company</t>
@@ -3706,96 +3706,9 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="H109" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>SettingsStorages</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>ХранилищеВариантовОтчетов</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G110" t="n">
-        <v>1024</v>
-      </c>
-      <c r="H110" t="n">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>WebServices</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>MAExchange</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>register.github@1c.ru</t>
-        </is>
-      </c>
-      <c r="G111" t="n">
-        <v>179</v>
-      </c>
-      <c r="H111" t="n">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>WebServices</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>MAExchange</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr"/>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>1C-Company</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>shan@1c.ru</t>
-        </is>
-      </c>
-      <c r="G112" t="n">
-        <v>177</v>
-      </c>
-      <c r="H112" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bugs and add html
</commit_message>
<xml_diff>
--- a/result/stats.xlsx
+++ b/result/stats.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H67"/>
+  <dimension ref="B2:H108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,14 +434,14 @@
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>1С:ГитКонвертер, ред. 1.0</t>
+          <t>Демонстрационное приложение</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Коммиты с 2016-01-01 по 2024-03-20</t>
+          <t>Коммиты с 2016-01-01 по 2024-03-21</t>
         </is>
       </c>
     </row>
@@ -492,59 +492,67 @@
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>Catalogs</t>
+          <t>AccumulationRegisters</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ВерсииХранилища</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>Взаиморасчеты</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Финансы</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1317</v>
+        <v>22</v>
       </c>
       <c r="H7" t="n">
-        <v>620</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>Catalogs</t>
+          <t>AccumulationRegisters</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ВерсииХранилища</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>Взаиморасчеты</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Финансы</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1445</v>
+        <v>52</v>
       </c>
       <c r="H8" t="n">
-        <v>1217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -555,25 +563,29 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>КопииХранилищКонфигурации</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>Встречи</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>623</v>
+        <v>771</v>
       </c>
       <c r="H9" t="n">
-        <v>571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -584,25 +596,29 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>КопииХранилищКонфигурации</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>ВходящиеПисьма</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>588</v>
+        <v>42</v>
       </c>
       <c r="H10" t="n">
-        <v>286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -613,25 +629,29 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ОчередиВыполнения</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>ИсходящиеПисьма</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>579</v>
+        <v>95</v>
       </c>
       <c r="H11" t="n">
-        <v>245</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -642,25 +662,29 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ОчередиВыполнения</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>ИсходящиеПисьма</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>570</v>
+        <v>271</v>
       </c>
       <c r="H12" t="n">
-        <v>482</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -671,25 +695,29 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ОчередиВыполнения</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>Контрагенты</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, Финансы</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Popov_MA</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>popma@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>16</v>
+        <v>391</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -700,25 +728,29 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ХранилищаКонфигураций</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>Контрагенты</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, Финансы</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>2741</v>
+        <v>62</v>
       </c>
       <c r="H14" t="n">
-        <v>835</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -729,22 +761,26 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ХранилищаКонфигураций</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
+          <t>МобильныеУстройства</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Бронников Владимир Сергеевич</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>vsbronnikov@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -758,25 +794,29 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ХранилищаКонфигураций</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
+          <t>НастройкиТорговогоОборудования</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>1857</v>
+        <v>4</v>
       </c>
       <c r="H16" t="n">
-        <v>1372</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -787,25 +827,29 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ХранилищаКонфигураций</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
+          <t>НастройкиТорговогоОборудования</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Завялик Павел Сергеевич</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>zavp@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="H17" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -816,25 +860,29 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ХранилищаКонфигураций</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+          <t>Организации</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Бахтиев Рамиз Ильгизович</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>bahr@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -845,22 +893,26 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ХранилищаКонфигураций</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
+          <t>Пользователи</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Popov_MA</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>popma@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -869,639 +921,707 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>Catalogs</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ДлительныеОперации</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
+          <t>РасчетныеСчетаКонтрагентов</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, Финансы</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>540</v>
+        <v>17</v>
       </c>
       <c r="H20" t="n">
-        <v>266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>Catalogs</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ДлительныеОперации</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
+          <t>Склады</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ТоварныеЗапасы</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>538</v>
+        <v>45</v>
       </c>
       <c r="H21" t="n">
-        <v>522</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>Catalogs</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ДлительныеОперацииКлиент</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>Товары</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, ТоварныеЗапасы</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="H22" t="n">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>Catalogs</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ДлительныеОперацииКлиент</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
+          <t>Товары</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, ТоварныеЗапасы</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>88</v>
+        <v>784</v>
       </c>
       <c r="H23" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>Catalogs</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
+          <t>ХранилищеВариантовОтчетов</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>9670</v>
+        <v>33</v>
       </c>
       <c r="H24" t="n">
-        <v>4799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>Catalogs</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+          <t>ХранимыеФайлы</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Ivan Maslikov</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>ivan.maslikov@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="H25" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>Catalogs</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
+          <t>ХранимыеФайлы</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Антон</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>33430119+BProg-Gladkov@users.noreply.github.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>3</v>
+        <v>1244</v>
       </c>
       <c r="H26" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonCommands</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
+          <t>НастроитьСканерШтрихКодов</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Закупки</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Andrei Ovsiankin</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>ovsiankin.aa@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonCommands</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
+          <t>ОбщиеНастройки</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Evgeny Zabelin</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>eug2603@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonCommands</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
+          <t>УстановитьВидимостьОбъектовЧерезODataAPI</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Бронников Владимир Сергеевич</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>vsbronnikov@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="H29" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonCommands</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
+          <t>УстановитьРасширениеРаботыСКриптографией</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Fenixnow</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>fenixnow@mail.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonCommands</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
+          <t>УстановитьРасширениеРаботыСФайлами</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>8420</v>
+        <v>9</v>
       </c>
       <c r="H31" t="n">
-        <v>6250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonCommands</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
+          <t>УстановитьСканерШтрихкодов</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Закупки</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Завялик Павел Сергеевич</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>zavp@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonCommands</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
+          <t>УстановитьСканерШтрихкодов</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Закупки</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Бахтиев Рамиз Ильгизович</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>bahr@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>204</v>
+        <v>12</v>
       </c>
       <c r="H33" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
+          <t>Звонок</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>ILazutin</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>lazutin.ilya@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H34" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>КонвертацияХранилища</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
+          <t>НастройкаPushУведомлений</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Vladislav Moroz</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>vlad.frost@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ОбработкаОчередей</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
+          <t>НастройкаPushУведомлений</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>459</v>
+        <v>68</v>
       </c>
       <c r="H36" t="n">
-        <v>181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ОбработкаОчередей</t>
+          <t>НастройкаПомощникаНеотработанныхЗаказов</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>370</v>
+        <v>69</v>
       </c>
       <c r="H37" t="n">
-        <v>353</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ОбщегоНазначения</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr"/>
+          <t>НастройкиМобильногоУстройства</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>753</v>
+        <v>144</v>
       </c>
       <c r="H38" t="n">
-        <v>329</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ОбщегоНазначения</t>
+          <t>ОбщиеНастройки</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>662</v>
+        <v>5</v>
       </c>
       <c r="H39" t="n">
-        <v>620</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияГлобальный</t>
+          <t>ФормаПодбора</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="H40" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>CommonModules</t>
+          <t>CommonForms</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияГлобальный</t>
+          <t>ФормаПодбораМобильная</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="H41" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1512,25 +1632,25 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияКлиент</t>
+          <t>ГеопозиционированиеКлиент</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>190</v>
+        <v>115</v>
       </c>
       <c r="H42" t="n">
-        <v>174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1541,25 +1661,25 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияКлиент</t>
+          <t>ГеопозиционированиеСервер</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>182</v>
+        <v>66</v>
       </c>
       <c r="H43" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1570,25 +1690,25 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияКлиентСервер</t>
+          <t>ОбменМобильныеОбщее</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>510</v>
+        <v>109</v>
       </c>
       <c r="H44" t="n">
-        <v>494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1599,25 +1719,25 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияКлиентСервер</t>
+          <t>ОбменМобильныеПереопределяемый</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>502</v>
+        <v>38</v>
       </c>
       <c r="H45" t="n">
-        <v>247</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46">
@@ -1628,25 +1748,25 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияПовтИсп</t>
+          <t>ОбменМобильныеПереопределяемый</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>497</v>
+        <v>238</v>
       </c>
       <c r="H46" t="n">
-        <v>246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1657,25 +1777,25 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ОбщегоНазначенияПовтИсп</t>
+          <t>Пользователи</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>474</v>
+        <v>43</v>
       </c>
       <c r="H47" t="n">
-        <v>426</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48">
@@ -1686,25 +1806,25 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>РаботаВБезопасномРежиме</t>
+          <t>Пользователи</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>500</v>
+        <v>64</v>
       </c>
       <c r="H48" t="n">
-        <v>484</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1715,25 +1835,25 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>РаботаВБезопасномРежиме</t>
+          <t>Помощник</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>492</v>
+        <v>244</v>
       </c>
       <c r="H49" t="n">
-        <v>242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1744,25 +1864,25 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>РегламентныеЗаданияСервер</t>
+          <t>ПомощникКлиент</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>482</v>
+        <v>24</v>
       </c>
       <c r="H50" t="n">
-        <v>466</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1773,25 +1893,25 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>РегламентныеЗаданияСервер</t>
+          <t>ПроведениеСервер</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>Арипов Никита</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>aripovn@gmail.com</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>940</v>
+        <v>3</v>
       </c>
       <c r="H51" t="n">
-        <v>466</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1802,25 +1922,25 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>РегламентныеЗаданияСлужебный</t>
+          <t>РаботаСДоставляемымиУведомлениям</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>1268</v>
+        <v>49</v>
       </c>
       <c r="H52" t="n">
-        <v>1252</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53">
@@ -1831,25 +1951,25 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>РегламентныеЗаданияСлужебный</t>
+          <t>РаботаСДоставляемымиУведомлениям</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>1260</v>
+        <v>76</v>
       </c>
       <c r="H53" t="n">
-        <v>627</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1860,25 +1980,25 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>СтандартныеПодсистемыСервер</t>
+          <t>РаботаСИсториейДанных</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>637</v>
+        <v>4</v>
       </c>
       <c r="H54" t="n">
-        <v>621</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1889,25 +2009,25 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>СтандартныеПодсистемыСервер</t>
+          <t>РаботаСПанельюЗадач</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>629</v>
+        <v>53</v>
       </c>
       <c r="H55" t="n">
-        <v>311</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -1918,25 +2038,25 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>СтроковыеФункцииКлиентСервер</t>
+          <t>РаботаСПолнотекстовымПоиском</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>438</v>
+        <v>18</v>
       </c>
       <c r="H56" t="n">
-        <v>422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1947,283 +2067,283 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>СтроковыеФункцииКлиентСервер</t>
+          <t>РаботаСПоследовательностями</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>Арипов Никита</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>aripovn@gmail.com</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>430</v>
+        <v>3</v>
       </c>
       <c r="H57" t="n">
-        <v>211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>Constants</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>ПутьКВерсиямПлатформыНаСервере</t>
+          <t>РаботаСПочтой</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="H58" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>Constants</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ПутьКВерсиямПлатформыНаСервере</t>
+          <t>РаботаСПочтой</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>30</v>
+        <v>346</v>
       </c>
       <c r="H59" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>Constants</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ПутьКВерсиямПлатформыНаСервере</t>
+          <t>РаботаСПочтойВызовСервера</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>ILazutin</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>lazutin.ilya@gmail.com</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>КонвертацияВФорматEDT</t>
+          <t>РаботаСТорговымОборудованием</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>1105</v>
+        <v>3</v>
       </c>
       <c r="H61" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>КонвертацияВФорматEDT</t>
+          <t>РаботаСТорговымОборудованием</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>2087</v>
+        <v>177</v>
       </c>
       <c r="H62" t="n">
-        <v>116</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>КонвертацияВФорматEDT</t>
+          <t>РаботаСХранилищемОбщихНастроек</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Завялик Павел Сергеевич</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>zavp@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H63" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>РегламентныеИФоновыеЗадания</t>
+          <t>РаботаСХранилищемОбщихНастроек</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>2862</v>
+        <v>56</v>
       </c>
       <c r="H64" t="n">
-        <v>2802</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>DataProcessors</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>РегламентныеИФоновыеЗадания</t>
+          <t>РегламентныеЗаданияАгрегатов</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>2833</v>
+        <v>6</v>
       </c>
       <c r="H65" t="n">
-        <v>1401</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="inlineStr">
         <is>
-          <t>InformationRegisters</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ИнформацияПользователей</t>
+          <t>РегламентныеЗаданияАгрегатов</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>marmyshev@gmail.com</t>
+          <t>shan@1c.ru</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2232,30 +2352,1335 @@
     <row r="67">
       <c r="B67" t="inlineStr">
         <is>
-          <t>InformationRegisters</t>
+          <t>CommonModules</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ИнформацияПользователей</t>
+          <t>СервисныеМеханизмы</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Dmitriy Marmyshev</t>
+          <t>1C-Company</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>dmar@1c.ru</t>
+          <t>register.github@1c.ru</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H67" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>CommonModules</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>СервисныеМеханизмы</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>11</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>CommonModules</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>УведомленияКлиент</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>60</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>CommonModules</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>УведомленияСервер</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>153</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>АдминистративныйСервис</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>13</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>ЖурналРегистрации</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ЖурналРегистрации</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>917</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>НастройкиПользователя</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>2</v>
+      </c>
+      <c r="H74" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>НастройкиПользователя</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>65</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>ПроведениеДокументов</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>151</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Путеводитель</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>43</v>
+      </c>
+      <c r="H77" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Путеводитель</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>191</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>СписокАктивныхПользователей</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>106</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>УдалениеПомеченныхОбъектов</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>284</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>УправлениеАгрегатамиПродаж</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>232</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>УправлениеНастройкамиФорм</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>415</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>УправлениеПолнотекстовымПоиском</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>88</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>УправлениеСистемойВзаимодействия</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>173</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>ЭлектроннаяПочта</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>17</v>
+      </c>
+      <c r="H85" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>DataProcessors</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ЭлектроннаяПочта</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>195</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Заказ</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Продажи</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>162</v>
+      </c>
+      <c r="H87" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Заказ</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Продажи</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>323</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>НовыйДокумент</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Арипов Никита</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>aripovn@gmail.com</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>6</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>ОперацияПоУчетуТоваров</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>ТоварныеЗапасы</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>23</v>
+      </c>
+      <c r="H90" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>ОперацияПоУчетуТоваров</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>ТоварныеЗапасы</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>90</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Оплата</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Финансы</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>7</v>
+      </c>
+      <c r="H92" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Оплата</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Финансы</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>89</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>ПоступлениеДенег</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Финансы</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>7</v>
+      </c>
+      <c r="H94" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>ПоступлениеДенег</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Финансы</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>85</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>ПриходТовара</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Закупки</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>58</v>
+      </c>
+      <c r="H96" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>ПриходТовара</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Закупки</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>242</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>РасходТовара</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Продажи</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>129</v>
+      </c>
+      <c r="H98" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>РасходТовара</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Продажи</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>688</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>ExchangePlans</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Мобильные</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Предприятие</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>13</v>
+      </c>
+      <c r="H100" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>HTTPServices</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>ОписанияТоваров</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>2</v>
+      </c>
+      <c r="H101" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>HTTPServices</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>ОписанияТоваров</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>67</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>HTTPServices</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Товары</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G103" t="n">
+        <v>2</v>
+      </c>
+      <c r="H103" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>HTTPServices</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Товары</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>216</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Reports</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>ОстаткиТоваровНаСкладах</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, ТоварныеЗапасы</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G105" t="n">
+        <v>1</v>
+      </c>
+      <c r="H105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Reports</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>ОстаткиТоваровНаСкладах</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Закупки, Продажи, ТоварныеЗапасы</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>8</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>SettingsStorages</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>ХранилищеВариантовОтчетов</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>shan@1c.ru</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>512</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>WebServices</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>MAExchange</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>1C-Company</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>register.github@1c.ru</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>179</v>
+      </c>
+      <c r="H108" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>